<commit_message>
update response options for gender+license
</commit_message>
<xml_diff>
--- a/survey-resources/data-xls/demo-survey-short-v1.xlsx
+++ b/survey-resources/data-xls/demo-survey-short-v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="190">
   <si>
     <t>type</t>
   </si>
@@ -87,10 +87,10 @@
     <t>What_is_your_gender</t>
   </si>
   <si>
-    <t>What is your gender?</t>
-  </si>
-  <si>
-    <t>¿Cuál es su género?</t>
+    <t>What best describes your gender?</t>
+  </si>
+  <si>
+    <t>¿Cuál describe de la mejor manera su género?</t>
   </si>
   <si>
     <t>select_multiple hw6ou02</t>
@@ -216,6 +216,15 @@
     <t>sj0gn93</t>
   </si>
   <si>
+    <t>woman</t>
+  </si>
+  <si>
+    <t>Woman</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
     <t>man</t>
   </si>
   <si>
@@ -225,22 +234,22 @@
     <t>Hombre</t>
   </si>
   <si>
-    <t>woman</t>
-  </si>
-  <si>
-    <t>Woman</t>
-  </si>
-  <si>
-    <t>Mujer</t>
-  </si>
-  <si>
-    <t>non_binary_genderqueer_gender_non_confor</t>
-  </si>
-  <si>
-    <t>Non-binary/genderqueer/gender non-conforming</t>
-  </si>
-  <si>
-    <t>No binaria / genderqueer / género no conforme</t>
+    <t>transgender</t>
+  </si>
+  <si>
+    <t>Transgender</t>
+  </si>
+  <si>
+    <t>Transgénero</t>
+  </si>
+  <si>
+    <t>non_binary</t>
+  </si>
+  <si>
+    <t>Non-binary</t>
+  </si>
+  <si>
+    <t>No binaria</t>
   </si>
   <si>
     <t>other</t>
@@ -1231,6 +1240,9 @@
       <c r="D3" t="s">
         <v>71</v>
       </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -1245,6 +1257,9 @@
       <c r="D4" t="s">
         <v>74</v>
       </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -1259,6 +1274,9 @@
       <c r="D5" t="s">
         <v>77</v>
       </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -1273,24 +1291,30 @@
       <c r="D6" t="s">
         <v>80</v>
       </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>81</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>82</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>83</v>
       </c>
-      <c r="D7" t="s">
-        <v>84</v>
+      <c r="E7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>85</v>
@@ -1304,7 +1328,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
         <v>88</v>
@@ -1318,7 +1342,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
         <v>91</v>
@@ -1332,7 +1356,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>94</v>
@@ -1346,7 +1370,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
         <v>97</v>
@@ -1360,7 +1384,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
         <v>100</v>
@@ -1374,7 +1398,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
         <v>103</v>
@@ -1388,21 +1412,21 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
         <v>78</v>
@@ -1416,21 +1440,21 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
         <v>110</v>
@@ -1439,133 +1463,133 @@
         <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D27" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1573,16 +1597,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -1590,16 +1614,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B29" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C29" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D29" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -1607,16 +1631,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B30" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E30">
         <v>4</v>
@@ -1624,16 +1648,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -1641,30 +1665,30 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B33" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C33" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D33" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1672,16 +1696,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C34" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D34" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -1689,16 +1713,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C35" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -1706,16 +1730,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B36" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C36" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D36" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -1723,16 +1747,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B37" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D37" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E37">
         <v>5</v>
@@ -1740,16 +1764,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E38">
         <v>6</v>
@@ -1757,212 +1781,212 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C39" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D39" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C40" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D40" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C41" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D41" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B42" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C42" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C43" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B44" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C44" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B45" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C46" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D46" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C48" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D48" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B49" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C49" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D49" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B50" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C50" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B51" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C51" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D51" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C52" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D52" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D53" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1980,30 +2004,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>